<commit_message>
bj: update onsho stop forms
</commit_message>
<xml_diff>
--- a/ONCHO/Impact Assessments/Benin/stop/bj_oncho_stop_2_202306_questions.xlsx
+++ b/ONCHO/Impact Assessments/Benin/stop/bj_oncho_stop_2_202306_questions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\ONCHO\Impact Assessments\Benin\stop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91072948-C5E4-463D-B834-38FAD591BE80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE3531DC-3F2C-4F61-9E73-AB1D710BE459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="261">
   <si>
     <t>form_title</t>
   </si>
@@ -520,15 +520,9 @@
     <t>Si oui, sur quelle partie du corps se situent les observations de l'onchocercose ?</t>
   </si>
   <si>
-    <t>(2023 Juin) ONCHO Stop TDM - 2. Questionnaire individuel</t>
-  </si>
-  <si>
     <t>string</t>
   </si>
   <si>
-    <t>bj_oncho_stop_2_202306_questions</t>
-  </si>
-  <si>
     <t>p_RecorderID</t>
   </si>
   <si>
@@ -797,6 +791,39 @@
   </si>
   <si>
     <t>. &lt;= ${p_age_yrs}</t>
+  </si>
+  <si>
+    <t>bj_oncho_stop_2_202306_questions_v1_2</t>
+  </si>
+  <si>
+    <t>Scanner</t>
+  </si>
+  <si>
+    <t>id_type</t>
+  </si>
+  <si>
+    <t>select_one id_type</t>
+  </si>
+  <si>
+    <t>p_id_type</t>
+  </si>
+  <si>
+    <t>Type d'identification</t>
+  </si>
+  <si>
+    <t>p_manual_id</t>
+  </si>
+  <si>
+    <t>${p_consent} = 'Oui' and ${p_id_type} = 'Scanner'</t>
+  </si>
+  <si>
+    <t>${p_consent} = 'Oui' and ${p_id_type} = 'Manuel'</t>
+  </si>
+  <si>
+    <t>Manuel</t>
+  </si>
+  <si>
+    <t>(2023 Juin) ONCHO Stop TDM - 2. Questionnaire individuel V1.2</t>
   </si>
 </sst>
 </file>
@@ -1312,13 +1339,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L66"/>
+  <dimension ref="A1:L68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
+      <selection pane="bottomRight" activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1380,7 +1407,7 @@
         <v>16</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>15</v>
@@ -1405,10 +1432,10 @@
     </row>
     <row r="3" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>31</v>
@@ -1427,10 +1454,10 @@
     </row>
     <row r="4" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>75</v>
@@ -1446,15 +1473,15 @@
       </c>
       <c r="K4" s="10"/>
       <c r="L4" s="11" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="5" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>93</v>
@@ -1470,7 +1497,7 @@
       </c>
       <c r="K5" s="10"/>
       <c r="L5" s="11" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="6" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1478,7 +1505,7 @@
         <v>21</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C6" s="17" t="s">
         <v>27</v>
@@ -1502,7 +1529,7 @@
         <v>80</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>81</v>
@@ -1524,7 +1551,7 @@
         <v>77</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>76</v>
@@ -1534,7 +1561,7 @@
       <c r="F8" s="6"/>
       <c r="G8" s="13"/>
       <c r="H8" s="30" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="I8" s="22"/>
       <c r="J8" s="23"/>
@@ -1546,7 +1573,7 @@
         <v>22</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>94</v>
@@ -1556,7 +1583,7 @@
       <c r="F9" s="6"/>
       <c r="G9" s="13"/>
       <c r="H9" s="30" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="I9" s="10"/>
       <c r="J9" s="6" t="s">
@@ -1567,20 +1594,20 @@
     </row>
     <row r="10" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>78</v>
+        <v>253</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>170</v>
+        <v>254</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>95</v>
+        <v>255</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="10"/>
       <c r="F10" s="6"/>
       <c r="G10" s="13"/>
       <c r="H10" s="30" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="I10" s="10"/>
       <c r="J10" s="6" t="s">
@@ -1589,22 +1616,22 @@
       <c r="K10" s="10"/>
       <c r="L10" s="10"/>
     </row>
-    <row r="11" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D11" s="9"/>
       <c r="E11" s="10"/>
       <c r="F11" s="6"/>
       <c r="G11" s="13"/>
       <c r="H11" s="30" t="s">
-        <v>223</v>
+        <v>257</v>
       </c>
       <c r="I11" s="10"/>
       <c r="J11" s="6" t="s">
@@ -1613,26 +1640,22 @@
       <c r="K11" s="10"/>
       <c r="L11" s="10"/>
     </row>
-    <row r="12" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>172</v>
+        <v>256</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="10"/>
-      <c r="F12" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="G12" s="13" t="s">
-        <v>87</v>
-      </c>
+      <c r="F12" s="6"/>
+      <c r="G12" s="13"/>
       <c r="H12" s="30" t="s">
-        <v>223</v>
+        <v>258</v>
       </c>
       <c r="I12" s="10"/>
       <c r="J12" s="6" t="s">
@@ -1641,22 +1664,22 @@
       <c r="K12" s="10"/>
       <c r="L12" s="10"/>
     </row>
-    <row r="13" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>16</v>
+        <v>85</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="10"/>
       <c r="F13" s="6"/>
       <c r="G13" s="13"/>
       <c r="H13" s="30" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="I13" s="10"/>
       <c r="J13" s="6" t="s">
@@ -1665,24 +1688,26 @@
       <c r="K13" s="10"/>
       <c r="L13" s="10"/>
     </row>
-    <row r="14" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="10"/>
       <c r="F14" s="6" t="s">
-        <v>251</v>
-      </c>
-      <c r="G14" s="13"/>
+        <v>86</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>87</v>
+      </c>
       <c r="H14" s="30" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="I14" s="10"/>
       <c r="J14" s="6" t="s">
@@ -1693,20 +1718,20 @@
     </row>
     <row r="15" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>92</v>
+        <v>16</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="10"/>
       <c r="F15" s="6"/>
       <c r="G15" s="13"/>
       <c r="H15" s="30" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I15" s="10"/>
       <c r="J15" s="6" t="s">
@@ -1715,22 +1740,24 @@
       <c r="K15" s="10"/>
       <c r="L15" s="10"/>
     </row>
-    <row r="16" spans="1:12" s="1" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>92</v>
+        <v>16</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="10"/>
-      <c r="F16" s="6"/>
+      <c r="F16" s="6" t="s">
+        <v>249</v>
+      </c>
       <c r="G16" s="13"/>
       <c r="H16" s="30" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="I16" s="10"/>
       <c r="J16" s="6" t="s">
@@ -1744,17 +1771,17 @@
         <v>92</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D17" s="9"/>
       <c r="E17" s="10"/>
       <c r="F17" s="6"/>
       <c r="G17" s="13"/>
       <c r="H17" s="30" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="I17" s="10"/>
       <c r="J17" s="6" t="s">
@@ -1763,22 +1790,22 @@
       <c r="K17" s="10"/>
       <c r="L17" s="10"/>
     </row>
-    <row r="18" spans="1:12" s="1" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" s="1" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>92</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D18" s="9"/>
       <c r="E18" s="10"/>
       <c r="F18" s="6"/>
       <c r="G18" s="13"/>
       <c r="H18" s="30" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="I18" s="10"/>
       <c r="J18" s="6" t="s">
@@ -1787,44 +1814,46 @@
       <c r="K18" s="10"/>
       <c r="L18" s="10"/>
     </row>
-    <row r="19" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>77</v>
+        <v>92</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>76</v>
+        <v>102</v>
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="10"/>
       <c r="F19" s="6"/>
       <c r="G19" s="13"/>
       <c r="H19" s="30" t="s">
-        <v>223</v>
-      </c>
-      <c r="I19" s="22"/>
-      <c r="J19" s="23"/>
+        <v>221</v>
+      </c>
+      <c r="I19" s="10"/>
+      <c r="J19" s="6" t="s">
+        <v>25</v>
+      </c>
       <c r="K19" s="10"/>
       <c r="L19" s="10"/>
     </row>
-    <row r="20" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" s="1" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>92</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D20" s="9"/>
       <c r="E20" s="10"/>
       <c r="F20" s="6"/>
       <c r="G20" s="13"/>
       <c r="H20" s="30" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="I20" s="10"/>
       <c r="J20" s="6" t="s">
@@ -1833,46 +1862,44 @@
       <c r="K20" s="10"/>
       <c r="L20" s="10"/>
     </row>
-    <row r="21" spans="1:12" s="1" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>111</v>
+        <v>77</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>105</v>
+        <v>76</v>
       </c>
       <c r="D21" s="9"/>
       <c r="E21" s="10"/>
       <c r="F21" s="6"/>
       <c r="G21" s="13"/>
       <c r="H21" s="30" t="s">
-        <v>227</v>
-      </c>
-      <c r="I21" s="10"/>
-      <c r="J21" s="6" t="s">
-        <v>25</v>
-      </c>
+        <v>221</v>
+      </c>
+      <c r="I21" s="22"/>
+      <c r="J21" s="23"/>
       <c r="K21" s="10"/>
       <c r="L21" s="10"/>
     </row>
-    <row r="22" spans="1:12" s="1" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>92</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="D22" s="9"/>
       <c r="E22" s="10"/>
       <c r="F22" s="6"/>
       <c r="G22" s="13"/>
       <c r="H22" s="30" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="I22" s="10"/>
       <c r="J22" s="6" t="s">
@@ -1883,20 +1910,20 @@
     </row>
     <row r="23" spans="1:12" s="1" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="D23" s="9"/>
       <c r="E23" s="10"/>
       <c r="F23" s="6"/>
       <c r="G23" s="13"/>
       <c r="H23" s="30" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="I23" s="10"/>
       <c r="J23" s="6" t="s">
@@ -1905,22 +1932,22 @@
       <c r="K23" s="10"/>
       <c r="L23" s="10"/>
     </row>
-    <row r="24" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" s="1" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>92</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D24" s="9"/>
       <c r="E24" s="10"/>
       <c r="F24" s="6"/>
       <c r="G24" s="13"/>
       <c r="H24" s="30" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="I24" s="10"/>
       <c r="J24" s="6" t="s">
@@ -1929,22 +1956,22 @@
       <c r="K24" s="10"/>
       <c r="L24" s="10"/>
     </row>
-    <row r="25" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" s="1" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>92</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D25" s="9"/>
       <c r="E25" s="10"/>
       <c r="F25" s="6"/>
       <c r="G25" s="13"/>
       <c r="H25" s="30" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="I25" s="10"/>
       <c r="J25" s="6" t="s">
@@ -1955,20 +1982,20 @@
     </row>
     <row r="26" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>22</v>
+        <v>92</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D26" s="9"/>
       <c r="E26" s="10"/>
       <c r="F26" s="6"/>
       <c r="G26" s="13"/>
       <c r="H26" s="30" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="I26" s="10"/>
       <c r="J26" s="6" t="s">
@@ -1977,22 +2004,22 @@
       <c r="K26" s="10"/>
       <c r="L26" s="10"/>
     </row>
-    <row r="27" spans="1:12" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>92</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D27" s="9"/>
       <c r="E27" s="10"/>
       <c r="F27" s="6"/>
       <c r="G27" s="13"/>
       <c r="H27" s="30" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="I27" s="10"/>
       <c r="J27" s="6" t="s">
@@ -2001,92 +2028,92 @@
       <c r="K27" s="10"/>
       <c r="L27" s="10"/>
     </row>
-    <row r="28" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>77</v>
+        <v>22</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>76</v>
+        <v>116</v>
       </c>
       <c r="D28" s="9"/>
       <c r="E28" s="10"/>
       <c r="F28" s="6"/>
       <c r="G28" s="13"/>
       <c r="H28" s="30" t="s">
-        <v>223</v>
-      </c>
-      <c r="I28" s="22"/>
-      <c r="J28" s="23"/>
+        <v>226</v>
+      </c>
+      <c r="I28" s="10"/>
+      <c r="J28" s="6" t="s">
+        <v>25</v>
+      </c>
       <c r="K28" s="10"/>
       <c r="L28" s="10"/>
     </row>
-    <row r="29" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="24" t="s">
+    <row r="29" spans="1:12" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="B29" s="25" t="s">
-        <v>189</v>
+      <c r="B29" s="16" t="s">
+        <v>185</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D29" s="9"/>
       <c r="E29" s="10"/>
       <c r="F29" s="6"/>
       <c r="G29" s="13"/>
-      <c r="H29" s="31" t="s">
-        <v>223</v>
-      </c>
-      <c r="I29" s="26"/>
-      <c r="J29" s="27" t="s">
+      <c r="H29" s="30" t="s">
+        <v>221</v>
+      </c>
+      <c r="I29" s="10"/>
+      <c r="J29" s="6" t="s">
         <v>25</v>
       </c>
       <c r="K29" s="10"/>
       <c r="L29" s="10"/>
     </row>
-    <row r="30" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="24" t="s">
-        <v>128</v>
-      </c>
-      <c r="B30" s="25" t="s">
-        <v>190</v>
+    <row r="30" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>186</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>127</v>
+        <v>76</v>
       </c>
       <c r="D30" s="9"/>
       <c r="E30" s="10"/>
       <c r="F30" s="6"/>
       <c r="G30" s="13"/>
-      <c r="H30" s="31" t="s">
-        <v>229</v>
-      </c>
-      <c r="I30" s="26"/>
-      <c r="J30" s="27" t="s">
-        <v>25</v>
-      </c>
+      <c r="H30" s="30" t="s">
+        <v>221</v>
+      </c>
+      <c r="I30" s="22"/>
+      <c r="J30" s="23"/>
       <c r="K30" s="10"/>
       <c r="L30" s="10"/>
     </row>
-    <row r="31" spans="1:12" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="24" t="s">
-        <v>22</v>
+        <v>92</v>
       </c>
       <c r="B31" s="25" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="D31" s="9"/>
       <c r="E31" s="10"/>
       <c r="F31" s="6"/>
       <c r="G31" s="13"/>
       <c r="H31" s="31" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="I31" s="26"/>
       <c r="J31" s="27" t="s">
@@ -2096,69 +2123,69 @@
       <c r="L31" s="10"/>
     </row>
     <row r="32" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A32" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="B32" s="16" t="s">
-        <v>192</v>
+      <c r="A32" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="B32" s="25" t="s">
+        <v>188</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D32" s="9"/>
       <c r="E32" s="10"/>
       <c r="F32" s="6"/>
       <c r="G32" s="13"/>
-      <c r="H32" s="30" t="s">
-        <v>223</v>
-      </c>
-      <c r="I32" s="10"/>
-      <c r="J32" s="6" t="s">
+      <c r="H32" s="31" t="s">
+        <v>227</v>
+      </c>
+      <c r="I32" s="26"/>
+      <c r="J32" s="27" t="s">
         <v>25</v>
       </c>
       <c r="K32" s="10"/>
       <c r="L32" s="10"/>
     </row>
-    <row r="33" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A33" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="B33" s="16" t="s">
-        <v>193</v>
+    <row r="33" spans="1:12" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A33" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B33" s="25" t="s">
+        <v>189</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D33" s="9"/>
       <c r="E33" s="10"/>
       <c r="F33" s="6"/>
       <c r="G33" s="13"/>
-      <c r="H33" s="30" t="s">
-        <v>231</v>
-      </c>
-      <c r="I33" s="10"/>
-      <c r="J33" s="6" t="s">
+      <c r="H33" s="31" t="s">
+        <v>228</v>
+      </c>
+      <c r="I33" s="26"/>
+      <c r="J33" s="27" t="s">
         <v>25</v>
       </c>
       <c r="K33" s="10"/>
       <c r="L33" s="10"/>
     </row>
-    <row r="34" spans="1:12" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>22</v>
+        <v>92</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D34" s="9"/>
       <c r="E34" s="10"/>
       <c r="F34" s="6"/>
       <c r="G34" s="13"/>
       <c r="H34" s="30" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
       <c r="I34" s="10"/>
       <c r="J34" s="6" t="s">
@@ -2167,70 +2194,70 @@
       <c r="K34" s="10"/>
       <c r="L34" s="10"/>
     </row>
-    <row r="35" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="B35" s="25" t="s">
-        <v>195</v>
+    <row r="35" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="B35" s="16" t="s">
+        <v>191</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D35" s="9"/>
       <c r="E35" s="10"/>
       <c r="F35" s="6"/>
       <c r="G35" s="13"/>
-      <c r="H35" s="31" t="s">
-        <v>223</v>
-      </c>
-      <c r="I35" s="26"/>
-      <c r="J35" s="27" t="s">
+      <c r="H35" s="30" t="s">
+        <v>229</v>
+      </c>
+      <c r="I35" s="10"/>
+      <c r="J35" s="6" t="s">
         <v>25</v>
       </c>
       <c r="K35" s="10"/>
       <c r="L35" s="10"/>
     </row>
-    <row r="36" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A36" s="24" t="s">
-        <v>128</v>
-      </c>
-      <c r="B36" s="25" t="s">
-        <v>196</v>
+    <row r="36" spans="1:12" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B36" s="16" t="s">
+        <v>192</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D36" s="9"/>
       <c r="E36" s="10"/>
       <c r="F36" s="6"/>
       <c r="G36" s="13"/>
-      <c r="H36" s="31" t="s">
-        <v>233</v>
-      </c>
-      <c r="I36" s="26"/>
-      <c r="J36" s="27" t="s">
+      <c r="H36" s="30" t="s">
+        <v>230</v>
+      </c>
+      <c r="I36" s="10"/>
+      <c r="J36" s="6" t="s">
         <v>25</v>
       </c>
       <c r="K36" s="10"/>
       <c r="L36" s="10"/>
     </row>
-    <row r="37" spans="1:12" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="24" t="s">
-        <v>22</v>
+        <v>92</v>
       </c>
       <c r="B37" s="25" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D37" s="9"/>
       <c r="E37" s="10"/>
       <c r="F37" s="6"/>
       <c r="G37" s="13"/>
       <c r="H37" s="31" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="I37" s="26"/>
       <c r="J37" s="27" t="s">
@@ -2240,69 +2267,69 @@
       <c r="L37" s="10"/>
     </row>
     <row r="38" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A38" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="B38" s="16" t="s">
-        <v>198</v>
+      <c r="A38" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="B38" s="25" t="s">
+        <v>194</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D38" s="9"/>
       <c r="E38" s="10"/>
       <c r="F38" s="6"/>
       <c r="G38" s="13"/>
-      <c r="H38" s="30" t="s">
-        <v>223</v>
-      </c>
-      <c r="I38" s="10"/>
-      <c r="J38" s="6" t="s">
+      <c r="H38" s="31" t="s">
+        <v>231</v>
+      </c>
+      <c r="I38" s="26"/>
+      <c r="J38" s="27" t="s">
         <v>25</v>
       </c>
       <c r="K38" s="10"/>
       <c r="L38" s="10"/>
     </row>
-    <row r="39" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A39" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="B39" s="16" t="s">
-        <v>199</v>
+    <row r="39" spans="1:12" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A39" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B39" s="25" t="s">
+        <v>195</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D39" s="9"/>
       <c r="E39" s="10"/>
       <c r="F39" s="6"/>
       <c r="G39" s="13"/>
-      <c r="H39" s="30" t="s">
-        <v>235</v>
-      </c>
-      <c r="I39" s="10"/>
-      <c r="J39" s="6" t="s">
+      <c r="H39" s="31" t="s">
+        <v>232</v>
+      </c>
+      <c r="I39" s="26"/>
+      <c r="J39" s="27" t="s">
         <v>25</v>
       </c>
       <c r="K39" s="10"/>
       <c r="L39" s="10"/>
     </row>
-    <row r="40" spans="1:12" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
-        <v>22</v>
+        <v>92</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D40" s="9"/>
       <c r="E40" s="10"/>
       <c r="F40" s="6"/>
       <c r="G40" s="13"/>
       <c r="H40" s="30" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
       <c r="I40" s="10"/>
       <c r="J40" s="6" t="s">
@@ -2312,69 +2339,69 @@
       <c r="L40" s="10"/>
     </row>
     <row r="41" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A41" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="B41" s="25" t="s">
-        <v>201</v>
+      <c r="A41" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="B41" s="16" t="s">
+        <v>197</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D41" s="9"/>
       <c r="E41" s="10"/>
       <c r="F41" s="6"/>
       <c r="G41" s="13"/>
-      <c r="H41" s="31" t="s">
-        <v>223</v>
-      </c>
-      <c r="I41" s="26"/>
-      <c r="J41" s="27" t="s">
+      <c r="H41" s="30" t="s">
+        <v>233</v>
+      </c>
+      <c r="I41" s="10"/>
+      <c r="J41" s="6" t="s">
         <v>25</v>
       </c>
       <c r="K41" s="10"/>
       <c r="L41" s="10"/>
     </row>
-    <row r="42" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A42" s="24" t="s">
-        <v>128</v>
-      </c>
-      <c r="B42" s="25" t="s">
-        <v>202</v>
+    <row r="42" spans="1:12" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A42" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B42" s="16" t="s">
+        <v>198</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D42" s="9"/>
       <c r="E42" s="10"/>
       <c r="F42" s="6"/>
       <c r="G42" s="13"/>
-      <c r="H42" s="31" t="s">
-        <v>237</v>
-      </c>
-      <c r="I42" s="26"/>
-      <c r="J42" s="27" t="s">
+      <c r="H42" s="30" t="s">
+        <v>234</v>
+      </c>
+      <c r="I42" s="10"/>
+      <c r="J42" s="6" t="s">
         <v>25</v>
       </c>
       <c r="K42" s="10"/>
       <c r="L42" s="10"/>
     </row>
-    <row r="43" spans="1:12" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A43" s="24" t="s">
-        <v>22</v>
+        <v>92</v>
       </c>
       <c r="B43" s="25" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D43" s="9"/>
       <c r="E43" s="10"/>
       <c r="F43" s="6"/>
       <c r="G43" s="13"/>
       <c r="H43" s="31" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="I43" s="26"/>
       <c r="J43" s="27" t="s">
@@ -2383,72 +2410,72 @@
       <c r="K43" s="10"/>
       <c r="L43" s="10"/>
     </row>
-    <row r="44" spans="1:12" s="1" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A44" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="B44" s="16" t="s">
-        <v>204</v>
+    <row r="44" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A44" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="B44" s="25" t="s">
+        <v>200</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="D44" s="28" t="s">
-        <v>144</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="D44" s="9"/>
       <c r="E44" s="10"/>
       <c r="F44" s="6"/>
       <c r="G44" s="13"/>
-      <c r="H44" s="30" t="s">
-        <v>223</v>
-      </c>
-      <c r="I44" s="10"/>
-      <c r="J44" s="6" t="s">
+      <c r="H44" s="31" t="s">
+        <v>235</v>
+      </c>
+      <c r="I44" s="26"/>
+      <c r="J44" s="27" t="s">
         <v>25</v>
       </c>
       <c r="K44" s="10"/>
       <c r="L44" s="10"/>
     </row>
-    <row r="45" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A45" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="B45" s="16" t="s">
-        <v>205</v>
+    <row r="45" spans="1:12" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A45" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B45" s="25" t="s">
+        <v>201</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="D45" s="9"/>
       <c r="E45" s="10"/>
       <c r="F45" s="6"/>
       <c r="G45" s="13"/>
-      <c r="H45" s="30" t="s">
-        <v>239</v>
-      </c>
-      <c r="I45" s="10"/>
-      <c r="J45" s="6" t="s">
+      <c r="H45" s="31" t="s">
+        <v>236</v>
+      </c>
+      <c r="I45" s="26"/>
+      <c r="J45" s="27" t="s">
         <v>25</v>
       </c>
       <c r="K45" s="10"/>
       <c r="L45" s="10"/>
     </row>
-    <row r="46" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" s="1" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
-        <v>22</v>
+        <v>92</v>
       </c>
       <c r="B46" s="16" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="D46" s="9"/>
+        <v>143</v>
+      </c>
+      <c r="D46" s="28" t="s">
+        <v>144</v>
+      </c>
       <c r="E46" s="10"/>
       <c r="F46" s="6"/>
       <c r="G46" s="13"/>
       <c r="H46" s="30" t="s">
-        <v>240</v>
+        <v>221</v>
       </c>
       <c r="I46" s="10"/>
       <c r="J46" s="6" t="s">
@@ -2457,72 +2484,72 @@
       <c r="K46" s="10"/>
       <c r="L46" s="10"/>
     </row>
-    <row r="47" spans="1:12" s="1" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A47" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="B47" s="25" t="s">
-        <v>207</v>
+    <row r="47" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A47" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="B47" s="16" t="s">
+        <v>203</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="D47" s="28" t="s">
-        <v>144</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="D47" s="9"/>
       <c r="E47" s="10"/>
       <c r="F47" s="6"/>
       <c r="G47" s="13"/>
-      <c r="H47" s="31" t="s">
-        <v>239</v>
-      </c>
-      <c r="I47" s="26"/>
-      <c r="J47" s="27" t="s">
+      <c r="H47" s="30" t="s">
+        <v>237</v>
+      </c>
+      <c r="I47" s="10"/>
+      <c r="J47" s="6" t="s">
         <v>25</v>
       </c>
       <c r="K47" s="10"/>
       <c r="L47" s="10"/>
     </row>
     <row r="48" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A48" s="24" t="s">
-        <v>128</v>
-      </c>
-      <c r="B48" s="25" t="s">
-        <v>208</v>
+      <c r="A48" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B48" s="16" t="s">
+        <v>204</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="D48" s="9"/>
       <c r="E48" s="10"/>
       <c r="F48" s="6"/>
       <c r="G48" s="13"/>
-      <c r="H48" s="31" t="s">
-        <v>241</v>
-      </c>
-      <c r="I48" s="26"/>
-      <c r="J48" s="27" t="s">
+      <c r="H48" s="30" t="s">
+        <v>238</v>
+      </c>
+      <c r="I48" s="10"/>
+      <c r="J48" s="6" t="s">
         <v>25</v>
       </c>
       <c r="K48" s="10"/>
       <c r="L48" s="10"/>
     </row>
-    <row r="49" spans="1:12" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" s="1" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A49" s="24" t="s">
-        <v>22</v>
+        <v>92</v>
       </c>
       <c r="B49" s="25" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="D49" s="9"/>
+        <v>146</v>
+      </c>
+      <c r="D49" s="28" t="s">
+        <v>144</v>
+      </c>
       <c r="E49" s="10"/>
       <c r="F49" s="6"/>
       <c r="G49" s="13"/>
       <c r="H49" s="31" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="I49" s="26"/>
       <c r="J49" s="27" t="s">
@@ -2532,47 +2559,45 @@
       <c r="L49" s="10"/>
     </row>
     <row r="50" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A50" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B50" s="16" t="s">
-        <v>210</v>
+      <c r="A50" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="B50" s="25" t="s">
+        <v>206</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="D50" s="28" t="s">
-        <v>149</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="D50" s="9"/>
       <c r="E50" s="10"/>
       <c r="F50" s="6"/>
       <c r="G50" s="13"/>
-      <c r="H50" s="30" t="s">
+      <c r="H50" s="31" t="s">
         <v>239</v>
       </c>
-      <c r="I50" s="10"/>
-      <c r="J50" s="6" t="s">
+      <c r="I50" s="26"/>
+      <c r="J50" s="27" t="s">
         <v>25</v>
       </c>
       <c r="K50" s="10"/>
       <c r="L50" s="10"/>
     </row>
-    <row r="51" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A51" s="24" t="s">
-        <v>92</v>
+        <v>22</v>
       </c>
       <c r="B51" s="25" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D51" s="9"/>
       <c r="E51" s="10"/>
       <c r="F51" s="6"/>
       <c r="G51" s="13"/>
       <c r="H51" s="31" t="s">
-        <v>223</v>
+        <v>240</v>
       </c>
       <c r="I51" s="26"/>
       <c r="J51" s="27" t="s">
@@ -2582,45 +2607,47 @@
       <c r="L51" s="10"/>
     </row>
     <row r="52" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A52" s="24" t="s">
-        <v>128</v>
-      </c>
-      <c r="B52" s="25" t="s">
-        <v>212</v>
+      <c r="A52" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B52" s="16" t="s">
+        <v>208</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="D52" s="9"/>
+        <v>148</v>
+      </c>
+      <c r="D52" s="28" t="s">
+        <v>149</v>
+      </c>
       <c r="E52" s="10"/>
       <c r="F52" s="6"/>
       <c r="G52" s="13"/>
-      <c r="H52" s="31" t="s">
-        <v>243</v>
-      </c>
-      <c r="I52" s="26"/>
-      <c r="J52" s="27" t="s">
+      <c r="H52" s="30" t="s">
+        <v>237</v>
+      </c>
+      <c r="I52" s="10"/>
+      <c r="J52" s="6" t="s">
         <v>25</v>
       </c>
       <c r="K52" s="10"/>
       <c r="L52" s="10"/>
     </row>
-    <row r="53" spans="1:12" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A53" s="24" t="s">
-        <v>22</v>
+        <v>92</v>
       </c>
       <c r="B53" s="25" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D53" s="9"/>
       <c r="E53" s="10"/>
       <c r="F53" s="6"/>
       <c r="G53" s="13"/>
       <c r="H53" s="31" t="s">
-        <v>244</v>
+        <v>221</v>
       </c>
       <c r="I53" s="26"/>
       <c r="J53" s="27" t="s">
@@ -2630,72 +2657,72 @@
       <c r="L53" s="10"/>
     </row>
     <row r="54" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A54" s="29" t="s">
-        <v>92</v>
-      </c>
-      <c r="B54" s="16" t="s">
-        <v>214</v>
+      <c r="A54" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="B54" s="25" t="s">
+        <v>210</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="D54" s="9"/>
       <c r="E54" s="10"/>
       <c r="F54" s="6"/>
       <c r="G54" s="13"/>
-      <c r="H54" s="30" t="s">
-        <v>223</v>
-      </c>
-      <c r="I54" s="10"/>
-      <c r="J54" s="6" t="s">
+      <c r="H54" s="31" t="s">
+        <v>241</v>
+      </c>
+      <c r="I54" s="26"/>
+      <c r="J54" s="27" t="s">
         <v>25</v>
       </c>
       <c r="K54" s="10"/>
       <c r="L54" s="10"/>
     </row>
-    <row r="55" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A55" s="29" t="s">
-        <v>128</v>
-      </c>
-      <c r="B55" s="32" t="s">
-        <v>215</v>
+    <row r="55" spans="1:12" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A55" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B55" s="25" t="s">
+        <v>211</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D55" s="9"/>
       <c r="E55" s="10"/>
       <c r="F55" s="6"/>
       <c r="G55" s="13"/>
-      <c r="H55" s="33" t="s">
-        <v>245</v>
-      </c>
-      <c r="I55" s="34"/>
-      <c r="J55" s="35" t="s">
+      <c r="H55" s="31" t="s">
+        <v>242</v>
+      </c>
+      <c r="I55" s="26"/>
+      <c r="J55" s="27" t="s">
         <v>25</v>
       </c>
       <c r="K55" s="10"/>
       <c r="L55" s="10"/>
     </row>
-    <row r="56" spans="1:12" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A56" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="B56" s="32" t="s">
-        <v>216</v>
+        <v>92</v>
+      </c>
+      <c r="B56" s="16" t="s">
+        <v>212</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D56" s="9"/>
       <c r="E56" s="10"/>
       <c r="F56" s="6"/>
       <c r="G56" s="13"/>
-      <c r="H56" s="33" t="s">
-        <v>246</v>
-      </c>
-      <c r="I56" s="34"/>
-      <c r="J56" s="35" t="s">
+      <c r="H56" s="30" t="s">
+        <v>221</v>
+      </c>
+      <c r="I56" s="10"/>
+      <c r="J56" s="6" t="s">
         <v>25</v>
       </c>
       <c r="K56" s="10"/>
@@ -2703,160 +2730,208 @@
     </row>
     <row r="57" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A57" s="29" t="s">
-        <v>92</v>
-      </c>
-      <c r="B57" s="16" t="s">
-        <v>217</v>
+        <v>128</v>
+      </c>
+      <c r="B57" s="32" t="s">
+        <v>213</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="D57" s="9"/>
       <c r="E57" s="10"/>
       <c r="F57" s="6"/>
       <c r="G57" s="13"/>
-      <c r="H57" s="30" t="s">
-        <v>223</v>
-      </c>
-      <c r="I57" s="10"/>
-      <c r="J57" s="6" t="s">
+      <c r="H57" s="33" t="s">
+        <v>243</v>
+      </c>
+      <c r="I57" s="34"/>
+      <c r="J57" s="35" t="s">
         <v>25</v>
       </c>
       <c r="K57" s="10"/>
       <c r="L57" s="10"/>
     </row>
-    <row r="58" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A58" s="24" t="s">
-        <v>128</v>
-      </c>
-      <c r="B58" s="25" t="s">
-        <v>218</v>
+    <row r="58" spans="1:12" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A58" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="B58" s="32" t="s">
+        <v>214</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D58" s="9"/>
       <c r="E58" s="10"/>
       <c r="F58" s="6"/>
       <c r="G58" s="13"/>
-      <c r="H58" s="31" t="s">
-        <v>247</v>
-      </c>
-      <c r="I58" s="26"/>
-      <c r="J58" s="27" t="s">
+      <c r="H58" s="33" t="s">
+        <v>244</v>
+      </c>
+      <c r="I58" s="34"/>
+      <c r="J58" s="35" t="s">
         <v>25</v>
       </c>
       <c r="K58" s="10"/>
       <c r="L58" s="10"/>
     </row>
-    <row r="59" spans="1:12" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A59" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="B59" s="25" t="s">
-        <v>219</v>
+    <row r="59" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A59" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="B59" s="16" t="s">
+        <v>215</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D59" s="9"/>
       <c r="E59" s="10"/>
       <c r="F59" s="6"/>
       <c r="G59" s="13"/>
-      <c r="H59" s="31" t="s">
-        <v>248</v>
-      </c>
-      <c r="I59" s="26"/>
-      <c r="J59" s="27" t="s">
+      <c r="H59" s="30" t="s">
+        <v>221</v>
+      </c>
+      <c r="I59" s="10"/>
+      <c r="J59" s="6" t="s">
         <v>25</v>
       </c>
       <c r="K59" s="10"/>
       <c r="L59" s="10"/>
     </row>
-    <row r="60" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B60" s="16" t="s">
-        <v>220</v>
+    <row r="60" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A60" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="B60" s="25" t="s">
+        <v>216</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="D60" s="9"/>
       <c r="E60" s="10"/>
       <c r="F60" s="6"/>
       <c r="G60" s="13"/>
-      <c r="H60" s="10"/>
-      <c r="I60" s="10"/>
-      <c r="J60" s="6"/>
+      <c r="H60" s="31" t="s">
+        <v>245</v>
+      </c>
+      <c r="I60" s="26"/>
+      <c r="J60" s="27" t="s">
+        <v>25</v>
+      </c>
       <c r="K60" s="10"/>
       <c r="L60" s="10"/>
     </row>
-    <row r="61" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="8"/>
-      <c r="B61" s="16"/>
-      <c r="C61" s="9"/>
+    <row r="61" spans="1:12" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A61" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B61" s="25" t="s">
+        <v>217</v>
+      </c>
+      <c r="C61" s="9" t="s">
+        <v>154</v>
+      </c>
       <c r="D61" s="9"/>
       <c r="E61" s="10"/>
       <c r="F61" s="6"/>
       <c r="G61" s="13"/>
-      <c r="H61" s="10"/>
-      <c r="I61" s="10"/>
-      <c r="J61" s="6"/>
+      <c r="H61" s="31" t="s">
+        <v>246</v>
+      </c>
+      <c r="I61" s="26"/>
+      <c r="J61" s="27" t="s">
+        <v>25</v>
+      </c>
       <c r="K61" s="10"/>
       <c r="L61" s="10"/>
     </row>
     <row r="62" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B62" s="16" t="s">
+        <v>218</v>
+      </c>
+      <c r="C62" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="D62" s="9"/>
+      <c r="E62" s="10"/>
+      <c r="F62" s="6"/>
+      <c r="G62" s="13"/>
+      <c r="H62" s="10"/>
+      <c r="I62" s="10"/>
+      <c r="J62" s="6"/>
+      <c r="K62" s="10"/>
+      <c r="L62" s="10"/>
+    </row>
+    <row r="63" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="8"/>
+      <c r="B63" s="16"/>
+      <c r="C63" s="9"/>
+      <c r="D63" s="9"/>
+      <c r="E63" s="10"/>
+      <c r="F63" s="6"/>
+      <c r="G63" s="13"/>
+      <c r="H63" s="10"/>
+      <c r="I63" s="10"/>
+      <c r="J63" s="6"/>
+      <c r="K63" s="10"/>
+      <c r="L63" s="10"/>
+    </row>
+    <row r="64" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B62" s="18" t="s">
-        <v>221</v>
-      </c>
-      <c r="C62" s="17"/>
-      <c r="D62" s="17"/>
-      <c r="E62" s="8"/>
-      <c r="F62" s="8"/>
-      <c r="G62" s="15"/>
-      <c r="H62" s="8"/>
-      <c r="I62" s="8"/>
-      <c r="J62" s="6"/>
-      <c r="K62" s="8"/>
-      <c r="L62" s="8"/>
-    </row>
-    <row r="63" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="8" t="s">
+      <c r="B64" s="18" t="s">
+        <v>219</v>
+      </c>
+      <c r="C64" s="17"/>
+      <c r="D64" s="17"/>
+      <c r="E64" s="8"/>
+      <c r="F64" s="8"/>
+      <c r="G64" s="15"/>
+      <c r="H64" s="8"/>
+      <c r="I64" s="8"/>
+      <c r="J64" s="6"/>
+      <c r="K64" s="8"/>
+      <c r="L64" s="8"/>
+    </row>
+    <row r="65" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B63" s="18" t="s">
-        <v>222</v>
-      </c>
-      <c r="C63" s="17"/>
-      <c r="D63" s="17"/>
-      <c r="E63" s="8"/>
-      <c r="F63" s="8"/>
-      <c r="G63" s="15"/>
-      <c r="H63" s="8"/>
-      <c r="I63" s="8"/>
-      <c r="J63" s="6"/>
-      <c r="K63" s="8"/>
-      <c r="L63" s="8"/>
-    </row>
-    <row r="64" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="4"/>
-      <c r="C64" s="4"/>
-      <c r="D64" s="4"/>
-    </row>
-    <row r="65" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="4"/>
-      <c r="C65" s="4"/>
-      <c r="D65" s="4"/>
-    </row>
-    <row r="66" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B66"/>
-      <c r="C66"/>
-      <c r="D66"/>
+      <c r="B65" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="C65" s="17"/>
+      <c r="D65" s="17"/>
+      <c r="E65" s="8"/>
+      <c r="F65" s="8"/>
+      <c r="G65" s="15"/>
+      <c r="H65" s="8"/>
+      <c r="I65" s="8"/>
+      <c r="J65" s="6"/>
+      <c r="K65" s="8"/>
+      <c r="L65" s="8"/>
+    </row>
+    <row r="66" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B66" s="4"/>
+      <c r="C66" s="4"/>
+      <c r="D66" s="4"/>
+    </row>
+    <row r="67" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="4"/>
+      <c r="C67" s="4"/>
+      <c r="D67" s="4"/>
+    </row>
+    <row r="68" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B68"/>
+      <c r="C68"/>
+      <c r="D68"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2866,11 +2941,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F67"/>
+  <dimension ref="A1:F69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A23" sqref="A23:XFD66"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3181,37 +3256,37 @@
       <c r="F21" s="20"/>
     </row>
     <row r="22" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="11"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
+      <c r="A22" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>251</v>
+      </c>
       <c r="D22" s="20"/>
       <c r="E22" s="20"/>
       <c r="F22" s="20"/>
     </row>
     <row r="23" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
-        <v>29</v>
+        <v>252</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>38</v>
+        <v>259</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>38</v>
+        <v>259</v>
       </c>
       <c r="D23" s="20"/>
       <c r="E23" s="20"/>
       <c r="F23" s="20"/>
     </row>
     <row r="24" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>39</v>
-      </c>
+      <c r="A24" s="11"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
       <c r="D24" s="20"/>
       <c r="E24" s="20"/>
       <c r="F24" s="20"/>
@@ -3221,10 +3296,10 @@
         <v>29</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="D25" s="20"/>
       <c r="E25" s="20"/>
@@ -3235,10 +3310,10 @@
         <v>29</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D26" s="20"/>
       <c r="E26" s="20"/>
@@ -3249,52 +3324,48 @@
         <v>29</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D27" s="20"/>
       <c r="E27" s="20"/>
       <c r="F27" s="20"/>
     </row>
     <row r="28" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="11"/>
-      <c r="B28" s="11"/>
-      <c r="C28" s="11"/>
+      <c r="A28" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>41</v>
+      </c>
       <c r="D28" s="20"/>
       <c r="E28" s="20"/>
       <c r="F28" s="20"/>
     </row>
     <row r="29" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="D29" s="20" t="s">
-        <v>38</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="D29" s="20"/>
       <c r="E29" s="20"/>
       <c r="F29" s="20"/>
     </row>
     <row r="30" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B30" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D30" s="20" t="s">
-        <v>39</v>
-      </c>
+      <c r="A30" s="11"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="20"/>
       <c r="E30" s="20"/>
       <c r="F30" s="20"/>
     </row>
@@ -3303,13 +3374,13 @@
         <v>18</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D31" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E31" s="20"/>
       <c r="F31" s="20"/>
@@ -3319,13 +3390,13 @@
         <v>18</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="D32" s="20" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="E32" s="20"/>
       <c r="F32" s="20"/>
@@ -3335,13 +3406,13 @@
         <v>18</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="E33" s="20"/>
       <c r="F33" s="20"/>
@@ -3351,10 +3422,10 @@
         <v>18</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D34" s="20" t="s">
         <v>30</v>
@@ -3367,13 +3438,13 @@
         <v>18</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D35" s="20" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="E35" s="20"/>
       <c r="F35" s="20"/>
@@ -3383,13 +3454,13 @@
         <v>18</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="D36" s="20" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="E36" s="20"/>
       <c r="F36" s="20"/>
@@ -3399,66 +3470,66 @@
         <v>18</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="D37" s="20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E37" s="20"/>
       <c r="F37" s="20"/>
     </row>
     <row r="38" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="11"/>
-      <c r="B38" s="11"/>
-      <c r="C38" s="11"/>
-      <c r="D38" s="20"/>
+      <c r="A38" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D38" s="20" t="s">
+        <v>41</v>
+      </c>
       <c r="E38" s="20"/>
       <c r="F38" s="20"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="D39" s="20"/>
-      <c r="E39" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="F39" s="19"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="B40" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="C40" s="11" t="s">
-        <v>58</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="D39" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="E39" s="20"/>
+      <c r="F39" s="20"/>
+    </row>
+    <row r="40" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="11"/>
+      <c r="B40" s="11"/>
+      <c r="C40" s="11"/>
       <c r="D40" s="20"/>
-      <c r="E40" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="F40" s="19"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
         <v>35</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D41" s="20"/>
       <c r="E41" s="20" t="s">
@@ -3471,14 +3542,14 @@
         <v>35</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="D42" s="20"/>
       <c r="E42" s="20" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="F42" s="19"/>
     </row>
@@ -3487,14 +3558,14 @@
         <v>35</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D43" s="20"/>
       <c r="E43" s="20" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="F43" s="19"/>
     </row>
@@ -3503,10 +3574,10 @@
         <v>35</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="D44" s="20"/>
       <c r="E44" s="20" t="s">
@@ -3519,10 +3590,10 @@
         <v>35</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="D45" s="20"/>
       <c r="E45" s="20" t="s">
@@ -3535,10 +3606,10 @@
         <v>35</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D46" s="20"/>
       <c r="E46" s="20" t="s">
@@ -3551,10 +3622,10 @@
         <v>35</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="D47" s="20"/>
       <c r="E47" s="20" t="s">
@@ -3567,14 +3638,14 @@
         <v>35</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D48" s="20"/>
       <c r="E48" s="20" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="F48" s="19"/>
     </row>
@@ -3583,14 +3654,14 @@
         <v>35</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D49" s="20"/>
       <c r="E49" s="20" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="F49" s="19"/>
     </row>
@@ -3599,14 +3670,14 @@
         <v>35</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D50" s="20"/>
       <c r="E50" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F50" s="19"/>
     </row>
@@ -3615,14 +3686,14 @@
         <v>35</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
       <c r="D51" s="20"/>
       <c r="E51" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F51" s="19"/>
     </row>
@@ -3631,10 +3702,10 @@
         <v>35</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D52" s="20"/>
       <c r="E52" s="20" t="s">
@@ -3647,10 +3718,10 @@
         <v>35</v>
       </c>
       <c r="B53" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C53" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D53" s="20"/>
       <c r="E53" s="20" t="s">
@@ -3663,14 +3734,14 @@
         <v>35</v>
       </c>
       <c r="B54" s="11" t="s">
-        <v>32</v>
+        <v>67</v>
       </c>
       <c r="C54" s="11" t="s">
-        <v>32</v>
+        <v>67</v>
       </c>
       <c r="D54" s="20"/>
       <c r="E54" s="20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F54" s="19"/>
     </row>
@@ -3679,14 +3750,14 @@
         <v>35</v>
       </c>
       <c r="B55" s="11" t="s">
-        <v>68</v>
+        <v>34</v>
       </c>
       <c r="C55" s="11" t="s">
-        <v>68</v>
+        <v>34</v>
       </c>
       <c r="D55" s="20"/>
       <c r="E55" s="20" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="F55" s="19"/>
     </row>
@@ -3695,14 +3766,14 @@
         <v>35</v>
       </c>
       <c r="B56" s="11" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="C56" s="11" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="D56" s="20"/>
       <c r="E56" s="20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F56" s="19"/>
     </row>
@@ -3711,14 +3782,14 @@
         <v>35</v>
       </c>
       <c r="B57" s="11" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="C57" s="11" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="D57" s="20"/>
       <c r="E57" s="20" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="F57" s="19"/>
     </row>
@@ -3727,10 +3798,10 @@
         <v>35</v>
       </c>
       <c r="B58" s="11" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="D58" s="20"/>
       <c r="E58" s="20" t="s">
@@ -3743,10 +3814,10 @@
         <v>35</v>
       </c>
       <c r="B59" s="11" t="s">
-        <v>70</v>
+        <v>46</v>
       </c>
       <c r="C59" s="11" t="s">
-        <v>70</v>
+        <v>46</v>
       </c>
       <c r="D59" s="20"/>
       <c r="E59" s="20" t="s">
@@ -3759,14 +3830,14 @@
         <v>35</v>
       </c>
       <c r="B60" s="11" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="C60" s="11" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D60" s="20"/>
       <c r="E60" s="20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F60" s="19"/>
     </row>
@@ -3775,14 +3846,14 @@
         <v>35</v>
       </c>
       <c r="B61" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C61" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D61" s="20"/>
       <c r="E61" s="20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F61" s="19"/>
     </row>
@@ -3791,10 +3862,10 @@
         <v>35</v>
       </c>
       <c r="B62" s="11" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="D62" s="20"/>
       <c r="E62" s="20" t="s">
@@ -3807,10 +3878,10 @@
         <v>35</v>
       </c>
       <c r="B63" s="11" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="C63" s="11" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="D63" s="20"/>
       <c r="E63" s="20" t="s">
@@ -3823,14 +3894,14 @@
         <v>35</v>
       </c>
       <c r="B64" s="11" t="s">
-        <v>72</v>
+        <v>44</v>
       </c>
       <c r="C64" s="11" t="s">
-        <v>72</v>
+        <v>44</v>
       </c>
       <c r="D64" s="20"/>
       <c r="E64" s="20" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="F64" s="19"/>
     </row>
@@ -3839,14 +3910,14 @@
         <v>35</v>
       </c>
       <c r="B65" s="11" t="s">
-        <v>73</v>
+        <v>48</v>
       </c>
       <c r="C65" s="11" t="s">
-        <v>73</v>
+        <v>48</v>
       </c>
       <c r="D65" s="20"/>
       <c r="E65" s="20" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="F65" s="19"/>
     </row>
@@ -3855,10 +3926,10 @@
         <v>35</v>
       </c>
       <c r="B66" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C66" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D66" s="20"/>
       <c r="E66" s="20" t="s">
@@ -3867,16 +3938,48 @@
       <c r="F66" s="19"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="11"/>
-      <c r="B67" s="11"/>
-      <c r="C67" s="11"/>
+      <c r="A67" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B67" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="C67" s="11" t="s">
+        <v>73</v>
+      </c>
       <c r="D67" s="20"/>
-      <c r="E67" s="20"/>
+      <c r="E67" s="20" t="s">
+        <v>47</v>
+      </c>
       <c r="F67" s="19"/>
     </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B68" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C68" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D68" s="20"/>
+      <c r="E68" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="F68" s="19"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="11"/>
+      <c r="B69" s="11"/>
+      <c r="C69" s="11"/>
+      <c r="D69" s="20"/>
+      <c r="E69" s="20"/>
+      <c r="F69" s="19"/>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A68:B78">
-    <sortCondition ref="B68:B78"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A70:B80">
+    <sortCondition ref="B70:B80"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3887,14 +3990,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -3913,10 +4016,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>159</v>
+        <v>260</v>
       </c>
       <c r="B2" t="s">
-        <v>161</v>
+        <v>250</v>
       </c>
       <c r="C2" t="s">
         <v>36</v>

</xml_diff>